<commit_message>
Ajustes na geracao de arquivos RPI
</commit_message>
<xml_diff>
--- a/Examples/Exemplo_RPI.xlsx
+++ b/Examples/Exemplo_RPI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elcio\dev\RegistroANS\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elcio\Dev\RegistroANS\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A279FB6D-4227-40E0-9FA7-61905715F7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5E55F1-91DD-4669-A4B1-73F61DF793BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,7 +469,7 @@
     <t>123456</t>
   </si>
   <si>
-    <t>12123123123412</t>
+    <t>56837718000191</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1351,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2523,7 +2525,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>